<commit_message>
Updates to remove bugs and document code
</commit_message>
<xml_diff>
--- a/tests/test_code/hx711_calibration_script/hx711_calibration_spreadsheet.xlsx
+++ b/tests/test_code/hx711_calibration_script/hx711_calibration_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Business\(2) Refills\Code\Github\refill_station_repository\tests\test_code\hx711_calibration_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F96EEA2-A681-4771-9C0A-149D3B2874FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A81F47-EF0A-44C3-B073-863F50564DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration Factor" sheetId="1" r:id="rId1"/>
@@ -1503,13 +1503,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>31231.666666666668</c:v>
+                  <c:v>28851.333333333332</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54387.333333333336</c:v>
+                  <c:v>63273.666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86681.666666666672</c:v>
+                  <c:v>99301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3868,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Y11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,12 +3977,12 @@
         <v>150</v>
       </c>
       <c r="U9" s="19">
-        <f>(31027+31213+31455)/3</f>
-        <v>31231.666666666668</v>
+        <f>(28556+28935+29063)/3</f>
+        <v>28851.333333333332</v>
       </c>
       <c r="W9">
         <f>SUM(U9:U11)/SUM(T9:T11)</f>
-        <v>191.44518518518521</v>
+        <v>212.69555555555556</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -4003,8 +4003,8 @@
         <v>300</v>
       </c>
       <c r="U10" s="19">
-        <f>(53939+54398+54825)/3</f>
-        <v>54387.333333333336</v>
+        <f>(63059+63370+63392)/3</f>
+        <v>63273.666666666664</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -4025,8 +4025,8 @@
         <v>450</v>
       </c>
       <c r="U11" s="19">
-        <f>(86332+86703+87010)/3</f>
-        <v>86681.666666666672</v>
+        <f>(99695+99211+98997)/3</f>
+        <v>99301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>